<commit_message>
Added formatting to column headers
</commit_message>
<xml_diff>
--- a/formatted_grades.xlsx
+++ b/formatted_grades.xlsx
@@ -7,11 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="US History" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="World History" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Economics" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Sociology" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="US History" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="World History" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Economics" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sociology" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -21,13 +20,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -50,8 +52,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -417,14 +420,643 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Student ID</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Miller</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Jessica</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>A411502</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Garcia</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Sarah</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>A264593</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Davis</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Jessica</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>A583929</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Garcia</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Robert</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>A720520</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Davis</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Robert</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>A167602</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Miller</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Jessica</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>A964785</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Johnson</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Jessica</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>A973821</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Williams</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Jessica</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>A168077</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Sarah</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>A906147</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Williams</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>James</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>A944981</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Garcia</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>A436358</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Garcia</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>A709025</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Johnson</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>A226508</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Sarah</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>A642508</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Williams</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Robert</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>A776697</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Johnson</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>A345105</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Jessica</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>A832461</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Johnson</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>James</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>A771469</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Williams</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Jessica</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>A642695</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Miller</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>James</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>A303780</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Jones</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Karen</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>A908192</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Johnson</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Karen</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>A915935</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Jessica</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>A953645</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Linda</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>A239606</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Miller</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>A376048</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Miller</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>A544176</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Williams</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>James</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>A207415</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Jones</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Sarah</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>A414782</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Jessica</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>A459429</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Garcia</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Sarah</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>A544532</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -435,31 +1067,37 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Last Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>First Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Student ID</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Grade</t>
         </is>
@@ -468,327 +1106,327 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Miller</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jessica</t>
+          <t>James</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>A411502</t>
+          <t>A224814</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>79</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Garcia</t>
+          <t>Miller</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Sarah</t>
+          <t>James</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>A264593</t>
+          <t>A721849</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Davis</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jessica</t>
+          <t>Sarah</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>A583929</t>
+          <t>A632891</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Garcia</t>
+          <t>Davis</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Robert</t>
+          <t>Jessica</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>A720520</t>
+          <t>A839154</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>87</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Davis</t>
+          <t>Garcia</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Robert</t>
+          <t>Linda</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>A167602</t>
+          <t>A654921</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>85</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Miller</t>
+          <t>Garcia</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Jessica</t>
+          <t>Linda</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>A964785</t>
+          <t>A456673</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Jessica</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>A973821</t>
+          <t>A861585</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>33</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Jessica</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>A168077</t>
+          <t>A401874</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>93</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Brown</t>
+          <t>Davis</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Sarah</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>A906147</t>
+          <t>A691594</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>78</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Jones</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>James</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>A944981</t>
+          <t>A828069</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Garcia</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Linda</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>A436358</t>
+          <t>A577802</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>97</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Garcia</t>
+          <t>Jones</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>A709025</t>
+          <t>A391741</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>58</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Linda</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>A226508</t>
+          <t>A315172</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>5</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Brown</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Sarah</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>A642508</t>
+          <t>A141349</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>87</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Jones</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Robert</t>
+          <t>Linda</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>A776697</t>
+          <t>A882585</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>27</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Jones</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Linda</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>A345105</t>
+          <t>A878730</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Garcia</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -798,111 +1436,111 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>A832461</t>
+          <t>A633066</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>James</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>A771469</t>
+          <t>A985522</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>18</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Davis</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Jessica</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>A642695</t>
+          <t>A191033</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Miller</t>
+          <t>Garcia</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>James</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>A303780</t>
+          <t>A810174</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Jones</t>
+          <t>Davis</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Karen</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>A908192</t>
+          <t>A315975</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>99</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Karen</t>
+          <t>Jessica</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>A915935</t>
+          <t>A615686</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24">
@@ -913,42 +1551,42 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Jessica</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>A953645</t>
+          <t>A137519</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Jones</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Linda</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>A239606</t>
+          <t>A515348</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Miller</t>
+          <t>Garcia</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -958,31 +1596,31 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>A376048</t>
+          <t>A882142</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>57</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Miller</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>A544176</t>
+          <t>A748660</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>17</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28">
@@ -993,56 +1631,56 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>James</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>A207415</t>
+          <t>A413567</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>3</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Jones</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Sarah</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>A414782</t>
+          <t>A202409</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>15</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Brown</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Jessica</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>A459429</t>
+          <t>A856819</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>66</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31">
@@ -1053,16 +1691,196 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Sarah</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>A544532</t>
+          <t>A930566</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>44</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Miller</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Robert</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>A794939</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>James</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>A973902</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>A178063</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Garcia</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Robert</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>A906827</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>A620696</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Davis</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Jessica</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>A911729</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Davis</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>James</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>A293408</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Williams</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Jessica</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>A606582</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Garcia</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Karen</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>A887613</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1083,24 +1901,30 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Last Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>First Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Student ID</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Grade</t>
         </is>
@@ -1109,107 +1933,107 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Miller</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>James</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>A224814</t>
+          <t>A524563</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>49</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Miller</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>James</t>
+          <t>Linda</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>A721849</t>
+          <t>A136756</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>19</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Brown</t>
+          <t>Miller</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Sarah</t>
+          <t>Karen</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>A632891</t>
+          <t>A506708</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Davis</t>
+          <t>Miller</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jessica</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>A839154</t>
+          <t>A923990</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>17</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Garcia</t>
+          <t>Davis</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Linda</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>A654921</t>
+          <t>A396362</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Garcia</t>
+          <t>Davis</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1219,77 +2043,77 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>A456673</t>
+          <t>A591499</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>77</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Sarah</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>A861585</t>
+          <t>A636971</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Sarah</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>A401874</t>
+          <t>A954763</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>67</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Davis</t>
+          <t>Miller</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Robert</t>
+          <t>Sarah</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>A691594</t>
+          <t>A602085</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Jones</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1299,97 +2123,97 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>A828069</t>
+          <t>A256211</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>57</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Garcia</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Linda</t>
+          <t>Karen</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>A577802</t>
+          <t>A315504</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>4</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Jones</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>James</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>A391741</t>
+          <t>A355334</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Miller</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Linda</t>
+          <t>Jessica</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>A315172</t>
+          <t>A840817</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Karen</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>A141349</t>
+          <t>A950177</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Jones</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1399,57 +2223,57 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>A882585</t>
+          <t>A556425</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>81</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Jones</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Linda</t>
+          <t>Jessica</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>A878730</t>
+          <t>A341776</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Garcia</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Jessica</t>
+          <t>Karen</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>A633066</t>
+          <t>A670267</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Davis</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1459,267 +2283,267 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>A985522</t>
+          <t>A197327</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>92</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Davis</t>
+          <t>Jones</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>James</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>A191033</t>
+          <t>A276469</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>87</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Garcia</t>
+          <t>Davis</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Karen</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>A810174</t>
+          <t>A560443</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>93</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Davis</t>
+          <t>Garcia</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Robert</t>
+          <t>James</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>A315975</t>
+          <t>A675960</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>19</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Brown</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Jessica</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>A615686</t>
+          <t>A150361</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Miller</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Robert</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>A137519</t>
+          <t>A951439</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>97</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Jones</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Robert</t>
+          <t>Karen</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>A515348</t>
+          <t>A658689</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Garcia</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>A882142</t>
+          <t>A848040</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>99</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Davis</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Jessica</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>A748660</t>
+          <t>A965437</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>37</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Garcia</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>James</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>A413567</t>
+          <t>A326210</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Miller</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Karen</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>A202409</t>
+          <t>A452023</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>92</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Miller</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Robert</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>A856819</t>
+          <t>A228761</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>90</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Garcia</t>
+          <t>Davis</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Sarah</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>A930566</t>
+          <t>A874638</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Miller</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Robert</t>
+          <t>Jessica</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>A794939</t>
+          <t>A774064</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1734,102 +2558,102 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>James</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>A973902</t>
+          <t>A801440</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>36</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Brown</t>
+          <t>Davis</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Linda</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>A178063</t>
+          <t>A271333</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>80</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Garcia</t>
+          <t>Miller</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Robert</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>A906827</t>
+          <t>A776097</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>10</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Brown</t>
+          <t>Miller</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>James</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>A620696</t>
+          <t>A301916</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>91</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Davis</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Jessica</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>A911729</t>
+          <t>A651544</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>51</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Davis</t>
+          <t>Garcia</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1839,37 +2663,37 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>A293408</t>
+          <t>A290581</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Davis</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Jessica</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>A606582</t>
+          <t>A220383</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>66</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Garcia</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1879,11 +2703,11 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>A887613</t>
+          <t>A222043</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>19</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1892,827 +2716,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D40"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Last Name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>First Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Student ID</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Grade</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Miller</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Michael</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>A524563</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Williams</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Linda</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>A136756</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Miller</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Karen</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>A506708</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Miller</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Robert</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>A923990</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Davis</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>John</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>A396362</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Davis</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Linda</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>A591499</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Johnson</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Sarah</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>A636971</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Smith</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Sarah</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>A954763</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Miller</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Sarah</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>A602085</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Robert</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>A256211</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Garcia</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Karen</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>A315504</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Johnson</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>James</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>A355334</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Miller</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Jessica</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>A840817</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Johnson</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Karen</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>A950177</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Williams</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Linda</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>A556425</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Williams</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Jessica</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>A341776</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Williams</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Karen</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>A670267</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Davis</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Robert</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>A197327</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Jones</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>James</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>A276469</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Davis</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Karen</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>A560443</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Garcia</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>James</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>A675960</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Williams</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Robert</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>A150361</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Miller</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>John</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>A951439</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Smith</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Karen</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>A658689</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Johnson</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Michael</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>A848040</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Davis</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Jessica</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>A965437</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Garcia</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>James</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>A326210</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Miller</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Karen</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>A452023</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Miller</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>John</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>A228761</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Davis</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Sarah</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>A874638</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Smith</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Jessica</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>A774064</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Robert</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>A801440</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Davis</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Linda</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>A271333</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Miller</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Michael</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>A776097</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Miller</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>James</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>A301916</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>John</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>A651544</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Garcia</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>James</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>A290581</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Davis</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>John</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>A220383</t>
-        </is>
-      </c>
-      <c r="D39" t="n">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Williams</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Karen</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>A222043</t>
-        </is>
-      </c>
-      <c r="D40" t="n">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2725,24 +2728,30 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Last Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>First Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Student ID</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Grade</t>
         </is>

</xml_diff>